<commit_message>
Khop so Bao Cao Phi Chuyen Khoan
</commit_message>
<xml_diff>
--- a/reporting_tool/trading_service/output/GiaoDichLuuKy/BaoCaoThang/10.2021/Báo cáo phí chuyển khoản 10.2021.xlsx
+++ b/reporting_tool/trading_service/output/GiaoDichLuuKy/BaoCaoThang/10.2021/Báo cáo phí chuyển khoản 10.2021.xlsx
@@ -531,7 +531,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="5">
-        <v>0</v>
+        <v>11700</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -545,7 +545,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="5">
-        <v>7371357.300000001</v>
+        <v>7148277.97051587</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -559,7 +559,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="5">
-        <v>3567536.7</v>
+        <v>3517249.673455395</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -573,7 +573,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="5">
-        <v>11049571.84012126</v>
+        <v>10926317.89091849</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -587,7 +587,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="5">
-        <v>3751869.6</v>
+        <v>3640201.440161694</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -615,7 +615,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="5">
-        <v>541890</v>
+        <v>537690</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -629,7 +629,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="5">
-        <v>0</v>
+        <v>3166283.696987225</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -643,7 +643,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="5">
-        <v>4576022.84001823</v>
+        <v>4040336.403926175</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -657,7 +657,7 @@
         <v>28</v>
       </c>
       <c r="D13" s="5">
-        <v>15192552.73534624</v>
+        <v>10185758.62754164</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -671,7 +671,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="5">
-        <v>2776926.9</v>
+        <v>2696374.240314188</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -685,7 +685,7 @@
         <v>30</v>
       </c>
       <c r="D15" s="5">
-        <v>9681635.941061474</v>
+        <v>9128358.856179321</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -723,7 +723,7 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="6">
-        <v>58509363.85654719</v>
+        <v>54998548.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>